<commit_message>
Add small textual changes to sec.3.3.2, and DP 6 accordingly
</commit_message>
<xml_diff>
--- a/TotalWords.xlsx
+++ b/TotalWords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulbrandt/Documents/Promotieonderzoek/Papers/2021_archSIOp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6A3C3A5-596D-2B42-989D-8163291CD616}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353AF6B8-B1DE-1846-9222-EB7892CC559E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5420" yWindow="2080" windowWidth="23000" windowHeight="14900" xr2:uid="{D78067DD-871A-CF46-B3D8-5095EB884DC8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>1 - intro</t>
   </si>
@@ -105,13 +105,27 @@
   </si>
   <si>
     <t>GRAND TOTAL</t>
+  </si>
+  <si>
+    <t>(200 per stuk = )</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="168" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -120,12 +134,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -137,13 +175,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -456,201 +506,217 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5366DA1-E7A6-ED46-8E8B-FADD157C1B7C}">
-  <dimension ref="A2:B26"/>
+  <dimension ref="A3:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2">
-        <v>325</v>
-      </c>
-    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>1601</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="4">
         <v>642</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="4">
         <v>1021</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="4">
         <v>1611</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="4">
         <v>404</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="4">
         <v>380</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="4">
         <v>525</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="4">
         <v>412</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="4">
         <v>464</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="4">
         <v>493</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="4">
         <v>426</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="4">
         <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="4">
         <v>893</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="4">
         <v>473</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="4">
         <v>658</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="4">
         <v>1775</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="4">
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="5"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="6">
         <f>SUM(B3:B21)</f>
         <v>11943</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="C24" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="7">
+        <f>B24*200</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="B25" s="5"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="6">
         <f>B23+(B24*200)</f>
         <v>12943</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="6">
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add approach to sec.1, incl image relating concerns, DPs and Viewpoint.
</commit_message>
<xml_diff>
--- a/TotalWords.xlsx
+++ b/TotalWords.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulbrandt/Documents/Promotieonderzoek/Papers/2021_archSIOp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353AF6B8-B1DE-1846-9222-EB7892CC559E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3C36D5-A6C3-7849-886F-B422D6C13A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5420" yWindow="2080" windowWidth="23000" windowHeight="14900" xr2:uid="{D78067DD-871A-CF46-B3D8-5095EB884DC8}"/>
+    <workbookView xWindow="32840" yWindow="1420" windowWidth="23000" windowHeight="14900" xr2:uid="{D78067DD-871A-CF46-B3D8-5095EB884DC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>1 - intro</t>
   </si>
@@ -44,27 +44,12 @@
     <t>2 - Anch</t>
   </si>
   <si>
-    <t>2.1 - Seman</t>
-  </si>
-  <si>
-    <t>2.2 - Hetor</t>
-  </si>
-  <si>
-    <t>2.3 - Coop</t>
-  </si>
-  <si>
     <t>3 - Spanning</t>
   </si>
   <si>
     <t>3.1 Data</t>
   </si>
   <si>
-    <t>3.2 Scala</t>
-  </si>
-  <si>
-    <t>3.3 Hitl</t>
-  </si>
-  <si>
     <t>3.3.1 Reconc</t>
   </si>
   <si>
@@ -83,31 +68,55 @@
     <t>3.4.2 Eng SC</t>
   </si>
   <si>
-    <t>5. Roadway</t>
-  </si>
-  <si>
-    <t>6 ISO42010</t>
-  </si>
-  <si>
-    <t>7 Related work</t>
-  </si>
-  <si>
-    <t>8 Discc &amp; Fut</t>
-  </si>
-  <si>
     <t>Abstract</t>
   </si>
   <si>
     <t>TOTAL text</t>
   </si>
   <si>
-    <t># Fig + tables</t>
-  </si>
-  <si>
     <t>GRAND TOTAL</t>
   </si>
   <si>
-    <t>(200 per stuk = )</t>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>3.3 Positioning Hitl</t>
+  </si>
+  <si>
+    <t># Fig + tables (200 per stuk)</t>
+  </si>
+  <si>
+    <t>2.1 Seman</t>
+  </si>
+  <si>
+    <t>2.2 Hetor</t>
+  </si>
+  <si>
+    <t>2.3 Coop</t>
+  </si>
+  <si>
+    <t>3.2 Support Scala</t>
+  </si>
+  <si>
+    <t>4 - Roadway</t>
+  </si>
+  <si>
+    <t>4.1 Formulating</t>
+  </si>
+  <si>
+    <t>4.2 Mediation</t>
+  </si>
+  <si>
+    <t>4.3 Data T/C/S</t>
+  </si>
+  <si>
+    <t>5 - ISO42010</t>
+  </si>
+  <si>
+    <t>6 - Related work</t>
+  </si>
+  <si>
+    <t>7 - Disc/Conc/FW</t>
   </si>
 </sst>
 </file>
@@ -116,9 +125,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="168" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -133,8 +142,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -161,12 +199,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -174,26 +218,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="lijn" xfId="2" xr:uid="{89B2CECE-066B-974B-838D-F58BD26751C3}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -506,220 +615,547 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5366DA1-E7A6-ED46-8E8B-FADD157C1B7C}">
-  <dimension ref="A3:D27"/>
+  <dimension ref="A2:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="10">
+        <v>44831</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="22">
+        <v>44875</v>
+      </c>
+      <c r="E2" s="14"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="31"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="6">
         <v>1601</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="7">
+        <f>B3</f>
+        <v>1601</v>
+      </c>
+      <c r="D3" s="23">
+        <v>1837</v>
+      </c>
+      <c r="E3" s="29">
+        <f>D3</f>
+        <v>1837</v>
+      </c>
+      <c r="F3" s="32"/>
+      <c r="G3" s="29">
+        <f>F3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="6">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="7">
+        <f>SUM(B4:B7)</f>
+        <v>3332</v>
+      </c>
+      <c r="D4" s="23">
+        <v>58</v>
+      </c>
+      <c r="E4" s="15">
+        <f>SUM(D4:D7)</f>
+        <v>3404</v>
+      </c>
+      <c r="F4" s="32"/>
+      <c r="G4" s="15">
+        <f>SUM(F4:F7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="6">
+        <v>642</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="23">
+        <v>634</v>
+      </c>
+      <c r="E5" s="16"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="16"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="6">
+        <v>1021</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="23">
+        <v>1023</v>
+      </c>
+      <c r="E6" s="16"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="6">
+        <v>1611</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="23">
+        <v>1689</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="16"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="B8" s="6">
+        <v>404</v>
+      </c>
+      <c r="C8" s="7">
+        <f>SUM(B8:B17)</f>
+        <v>4507</v>
+      </c>
+      <c r="D8" s="23">
+        <v>402</v>
+      </c>
+      <c r="E8" s="15">
+        <f>SUM(D8:D17)</f>
+        <v>4955</v>
+      </c>
+      <c r="F8" s="32"/>
+      <c r="G8" s="15">
+        <f>SUM(F8:F17)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="4">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="B9" s="6">
+        <v>380</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="23">
+        <v>385</v>
+      </c>
+      <c r="E9" s="16"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="16"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="6">
+        <v>525</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="23">
+        <v>524</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="16"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="6">
+        <v>412</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="23">
+        <v>421</v>
+      </c>
+      <c r="E11" s="16"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="4">
-        <v>1611</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="B12" s="6">
+        <v>464</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="23">
+        <v>733</v>
+      </c>
+      <c r="E12" s="16"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="16"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="4">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="B13" s="6">
+        <v>493</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="23">
+        <v>401</v>
+      </c>
+      <c r="E13" s="16"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="16"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="4">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="B14" s="6">
+        <v>426</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="23">
+        <v>666</v>
+      </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="16"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="4">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="B15" s="6">
+        <v>37</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="23">
+        <v>37</v>
+      </c>
+      <c r="E15" s="16"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="16"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="4">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="B16" s="6">
+        <v>893</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="23">
+        <v>990</v>
+      </c>
+      <c r="E16" s="16"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="16"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="4">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="B17" s="6">
+        <v>473</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="23">
+        <v>396</v>
+      </c>
+      <c r="E17" s="16"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="16"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="6">
+        <v>658</v>
+      </c>
+      <c r="C18" s="7">
+        <f>SUM(B18:B21)</f>
+        <v>658</v>
+      </c>
+      <c r="D18" s="23">
+        <v>107</v>
+      </c>
+      <c r="E18" s="15">
+        <f>SUM(D18:D21)</f>
+        <v>1908</v>
+      </c>
+      <c r="F18" s="32"/>
+      <c r="G18" s="15">
+        <f>SUM(F18:F21)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="6">
+        <v>0</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="23">
+        <v>650</v>
+      </c>
+      <c r="E19" s="16"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="16"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="23">
+        <v>489</v>
+      </c>
+      <c r="E20" s="16"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="16"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="6">
+        <v>0</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="23">
+        <v>662</v>
+      </c>
+      <c r="E21" s="16"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="16"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="6">
+        <v>0</v>
+      </c>
+      <c r="C22" s="7">
+        <f>B22</f>
+        <v>0</v>
+      </c>
+      <c r="D22" s="23">
+        <v>0</v>
+      </c>
+      <c r="E22" s="15">
+        <f>D22</f>
+        <v>0</v>
+      </c>
+      <c r="F22" s="32"/>
+      <c r="G22" s="15">
+        <f>F22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="6">
+        <v>1775</v>
+      </c>
+      <c r="C23" s="7">
+        <f>B23</f>
+        <v>1775</v>
+      </c>
+      <c r="D23" s="23">
+        <v>2203</v>
+      </c>
+      <c r="E23" s="15">
+        <f>D23</f>
+        <v>2203</v>
+      </c>
+      <c r="F23" s="32"/>
+      <c r="G23" s="15">
+        <f>F23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="6">
+        <v>70</v>
+      </c>
+      <c r="C24" s="7">
+        <f>B24</f>
+        <v>70</v>
+      </c>
+      <c r="D24" s="23">
+        <v>883</v>
+      </c>
+      <c r="E24" s="15">
+        <f>D24</f>
+        <v>883</v>
+      </c>
+      <c r="F24" s="32"/>
+      <c r="G24" s="15">
+        <f>F24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="17"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="12">
+        <f>SUM(B3:B24)</f>
+        <v>11943</v>
+      </c>
+      <c r="C26" s="13">
+        <f>SUM(C3:C24)</f>
+        <v>11943</v>
+      </c>
+      <c r="D26" s="25">
+        <f t="shared" ref="D26" si="0">SUM(D3:D24)</f>
+        <v>15190</v>
+      </c>
+      <c r="E26" s="18">
+        <f t="shared" ref="C26:F26" si="1">SUM(E3:E24)</f>
+        <v>15190</v>
+      </c>
+      <c r="F26" s="34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="18">
+        <f t="shared" ref="G26" si="2">SUM(G3:G24)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="6">
+        <v>5</v>
+      </c>
+      <c r="C27" s="9">
+        <f>B27*200</f>
+        <v>1000</v>
+      </c>
+      <c r="D27" s="26">
+        <v>5</v>
+      </c>
+      <c r="E27" s="19">
+        <f>D27*200</f>
+        <v>1000</v>
+      </c>
+      <c r="F27" s="35"/>
+      <c r="G27" s="19">
+        <f>F27*200</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="20"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="12">
+        <f>B26+B28</f>
+        <v>11943</v>
+      </c>
+      <c r="C29" s="13">
+        <f>SUM(C26:C28)</f>
+        <v>12943</v>
+      </c>
+      <c r="D29" s="25">
+        <f>D26+D28</f>
+        <v>15190</v>
+      </c>
+      <c r="E29" s="18">
+        <f>SUM(E26:E28)</f>
+        <v>16190</v>
+      </c>
+      <c r="F29" s="34">
+        <f t="shared" ref="D29:F29" si="3">F26+F28</f>
+        <v>0</v>
+      </c>
+      <c r="G29" s="18">
+        <f>SUM(G26:G28)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="4">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="4">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="4">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="4">
-        <v>893</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="4">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="4">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" s="4">
-        <v>1775</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="4">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="B22" s="5"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="6">
-        <f>SUM(B3:B21)</f>
-        <v>11943</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24" s="4">
-        <v>5</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="7">
-        <f>B24*200</f>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-      <c r="B25" s="5"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="6">
-        <f>B23+(B24*200)</f>
-        <v>12943</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="6">
+      <c r="B30" s="8">
         <v>325</v>
       </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="28">
+        <v>331</v>
+      </c>
+      <c r="E30" s="21"/>
+      <c r="F30" s="37"/>
+      <c r="G30" s="21"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:G2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>